<commit_message>
new:displaying the age in years under the contact name
</commit_message>
<xml_diff>
--- a/config/forms/contact/person-create.xlsx
+++ b/config/forms/contact/person-create.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="149">
   <si>
     <t>type</t>
   </si>
@@ -204,7 +204,7 @@
     <t>date</t>
   </si>
   <si>
-    <t>birth</t>
+    <t>date_of_birth</t>
   </si>
   <si>
     <t>Date of Birth</t>
@@ -249,17 +249,10 @@
     <t>Marital Status</t>
   </si>
   <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>not</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We’d like you to choose a secret word that will become a passcode. We will ask you to text us this word before we can call you to chat with you. What word would you like to select? 
-</t>
-  </si>
-  <si>
     <t>meta</t>
+  </si>
+  <si>
+    <t>multiline</t>
   </si>
   <si>
     <t>created_by</t>
@@ -857,7 +850,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="20.25"/>
     <col customWidth="1" min="2" max="2" width="22.0"/>
-    <col customWidth="1" min="3" max="3" width="21.75"/>
+    <col customWidth="1" min="3" max="3" width="45.25"/>
     <col customWidth="1" min="7" max="7" width="44.63"/>
     <col customWidth="1" min="8" max="8" width="24.0"/>
     <col customWidth="1" min="10" max="10" width="35.63"/>
@@ -1273,26 +1266,34 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="3" t="s">
+    </row>
+    <row r="32">
+      <c r="A32" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="18" t="s">
+      <c r="C32" s="3"/>
+      <c r="E32" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="H32" s="7"/>
     </row>
     <row r="33">
       <c r="A33" s="15" t="s">
@@ -1321,25 +1322,12 @@
       <c r="H34" s="7"/>
     </row>
     <row r="35">
-      <c r="A35" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35" s="3"/>
-      <c r="G35" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="H35" s="7"/>
+      <c r="A35" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1363,7 +1351,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1374,266 +1362,266 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>121</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>128</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1658,22 +1646,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="22" t="s">
         <v>144</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>146</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="22"/>
@@ -1683,21 +1671,21 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C2" s="23" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-07-19_10-13</v>
+        <v>2022-07-19_20-20</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G2" s="7"/>
     </row>

</xml_diff>

<commit_message>
auto:fine tunning the enrollment and contact forms according to the new design changes
</commit_message>
<xml_diff>
--- a/config/forms/contact/person-create.xlsx
+++ b/config/forms/contact/person-create.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="134">
   <si>
     <t>type</t>
   </si>
@@ -138,16 +138,22 @@
     <t xml:space="preserve">string </t>
   </si>
   <si>
-    <t>Name</t>
+    <t>First Name</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
     <t>aka</t>
   </si>
   <si>
-    <t>Also Known As:</t>
+    <t>Also Known as:</t>
   </si>
   <si>
     <t>integer</t>
@@ -159,6 +165,12 @@
     <t>Docket Number</t>
   </si>
   <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Current Address</t>
+  </si>
+  <si>
     <t>tel</t>
   </si>
   <si>
@@ -202,12 +214,6 @@
   </si>
   <si>
     <t>Date of birth cannot be in the future</t>
-  </si>
-  <si>
-    <t>digital</t>
-  </si>
-  <si>
-    <t>Age in years at today’s Enrollment in the digital device:</t>
   </si>
   <si>
     <t>select_one sex</t>
@@ -1088,147 +1094,143 @@
       <c r="C20" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="F20" s="3"/>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="3" t="s">
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="5" t="s">
+      <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="3" t="s">
+    </row>
+    <row r="23">
+      <c r="A23" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I22" s="3" t="b">
+      <c r="C23" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="J22" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="3" t="s">
+      <c r="J24" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="J27" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="3" t="s">
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="17" t="s">
+      <c r="B30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="B31" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="3"/>
       <c r="E31" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="H31" s="7"/>
     </row>
     <row r="32">
       <c r="A32" s="15" t="s">
@@ -1238,6 +1240,9 @@
         <v>78</v>
       </c>
       <c r="C32" s="3"/>
+      <c r="E32" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="G32" s="7" t="s">
         <v>79</v>
       </c>
@@ -1257,12 +1262,25 @@
       <c r="H33" s="7"/>
     </row>
     <row r="34">
-      <c r="A34" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A34" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="G34" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H34" s="7"/>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1286,7 +1304,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1297,200 +1315,200 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20">
@@ -1545,22 +1563,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="22"/>
@@ -1570,21 +1588,21 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C2" s="23" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-07-25_10-04</v>
+        <v>2022-08-02_13-59</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G2" s="7"/>
     </row>

</xml_diff>

<commit_message>
auto:make the phone number to appear in the contact summary
</commit_message>
<xml_diff>
--- a/config/forms/contact/person-create.xlsx
+++ b/config/forms/contact/person-create.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="133">
   <si>
     <t>type</t>
   </si>
@@ -174,7 +174,7 @@
     <t>tel</t>
   </si>
   <si>
-    <t>telephone</t>
+    <t>phone</t>
   </si>
   <si>
     <t>Cell number</t>
@@ -268,9 +268,6 @@
   </si>
   <si>
     <t>list_name</t>
-  </si>
-  <si>
-    <t>phone</t>
   </si>
   <si>
     <t>banger</t>
@@ -1315,200 +1312,200 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>115</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="C17" s="21" t="s">
         <v>118</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B18" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>120</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B19" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="21" t="s">
         <v>122</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="20">
@@ -1563,22 +1560,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="22" t="s">
         <v>128</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>129</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="22"/>
@@ -1588,21 +1585,21 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>130</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>131</v>
       </c>
       <c r="C2" s="23" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-08-02_13-59</v>
+        <v>2022-09-15_23-49</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>133</v>
       </c>
       <c r="G2" s="7"/>
     </row>

</xml_diff>

<commit_message>
auto:adding new fields in the enrollment form
</commit_message>
<xml_diff>
--- a/config/forms/contact/person-create.xlsx
+++ b/config/forms/contact/person-create.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="121">
   <si>
     <t>type</t>
   </si>
@@ -165,6 +165,12 @@
     <t>Docket Number</t>
   </si>
   <si>
+    <t>tsis</t>
+  </si>
+  <si>
+    <t>TSIS number</t>
+  </si>
+  <si>
     <t>address</t>
   </si>
   <si>
@@ -183,6 +189,9 @@
     <t>Please enter a valid local number, or use the standard international format, which includes a plus sign (+) and country code. For example: +254712345678</t>
   </si>
   <si>
+    <t>Must be in the format +1 (876) xxx-xxx</t>
+  </si>
+  <si>
     <t>select_one phone</t>
   </si>
   <si>
@@ -192,13 +201,13 @@
     <t>Type of phone</t>
   </si>
   <si>
-    <t>select_one message</t>
-  </si>
-  <si>
-    <t>cell</t>
-  </si>
-  <si>
-    <t>Is it okay to leave a message on your cell phone?</t>
+    <t>select_one network</t>
+  </si>
+  <si>
+    <t>network1</t>
+  </si>
+  <si>
+    <t>Which network do you use?</t>
   </si>
   <si>
     <t>date</t>
@@ -232,15 +241,6 @@
   </si>
   <si>
     <t>Gender Identity</t>
-  </si>
-  <si>
-    <t>select_one status</t>
-  </si>
-  <si>
-    <t>stat</t>
-  </si>
-  <si>
-    <t>Marital Status</t>
   </si>
   <si>
     <t>meta</t>
@@ -284,18 +284,6 @@
 </t>
   </si>
   <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>sex</t>
   </si>
   <si>
@@ -326,45 +314,6 @@
     <t>gender_female</t>
   </si>
   <si>
-    <t xml:space="preserve">status </t>
-  </si>
-  <si>
-    <t>single</t>
-  </si>
-  <si>
-    <t>Single</t>
-  </si>
-  <si>
-    <t>married</t>
-  </si>
-  <si>
-    <t>Married</t>
-  </si>
-  <si>
-    <t>separated</t>
-  </si>
-  <si>
-    <t>Separated</t>
-  </si>
-  <si>
-    <t>divorced</t>
-  </si>
-  <si>
-    <t>Divorced</t>
-  </si>
-  <si>
-    <t>widowed</t>
-  </si>
-  <si>
-    <t>Widowed</t>
-  </si>
-  <si>
-    <t>common</t>
-  </si>
-  <si>
-    <t>Common-Law</t>
-  </si>
-  <si>
     <t>place_type</t>
   </si>
   <si>
@@ -384,6 +333,21 @@
   </si>
   <si>
     <t>Area</t>
+  </si>
+  <si>
+    <t>network</t>
+  </si>
+  <si>
+    <t>digicel</t>
+  </si>
+  <si>
+    <t>Digicel</t>
+  </si>
+  <si>
+    <t>flow</t>
+  </si>
+  <si>
+    <t>Flow</t>
   </si>
   <si>
     <t>form_title</t>
@@ -503,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -561,14 +525,20 @@
     <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -805,7 +775,8 @@
     <col customWidth="1" min="3" max="3" width="45.25"/>
     <col customWidth="1" min="7" max="7" width="44.63"/>
     <col customWidth="1" min="8" max="8" width="24.0"/>
-    <col customWidth="1" min="10" max="10" width="35.63"/>
+    <col customWidth="1" min="10" max="10" width="116.25"/>
+    <col customWidth="1" min="11" max="11" width="29.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1114,10 +1085,13 @@
       <c r="C22" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="F22" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>50</v>
@@ -1128,29 +1102,35 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="3" t="s">
+    </row>
+    <row r="25">
+      <c r="A25" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I24" s="3" t="b">
+      <c r="B25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="J24" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="J25" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="K25" s="3" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1175,21 +1155,21 @@
       <c r="C27" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="J28" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1312,7 +1292,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>85</v>
@@ -1323,7 +1303,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>87</v>
@@ -1337,10 +1317,10 @@
         <v>89</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5">
@@ -1348,15 +1328,15 @@
         <v>89</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>94</v>
@@ -1367,176 +1347,100 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>97</v>
+      <c r="C10" s="20" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="20" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="22" t="s">
         <v>107</v>
       </c>
+      <c r="C12" s="23" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="A13" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>109</v>
       </c>
+      <c r="C13" s="23" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="A14" s="7"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>113</v>
-      </c>
+      <c r="A15" s="7"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>115</v>
-      </c>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="7"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="7"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="7"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="7"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1560,46 +1464,46 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>128</v>
+        <v>115</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>116</v>
       </c>
       <c r="G1" s="8"/>
-      <c r="H1" s="22"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="8"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="23" t="str">
+        <v>118</v>
+      </c>
+      <c r="C2" s="25" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-09-15_23-49</v>
+        <v>2022-09-29_11-31</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="G2" s="7"/>
     </row>

</xml_diff>

<commit_message>
auto:updates in the enrollment form fields
</commit_message>
<xml_diff>
--- a/config/forms/contact/person-create.xlsx
+++ b/config/forms/contact/person-create.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="125">
   <si>
     <t>type</t>
   </si>
@@ -177,19 +177,25 @@
     <t>Current Address</t>
   </si>
   <si>
+    <t>address1</t>
+  </si>
+  <si>
+    <t>Previous Address</t>
+  </si>
+  <si>
     <t>tel</t>
   </si>
   <si>
     <t>phone</t>
   </si>
   <si>
-    <t>Cell number</t>
+    <t>Current Cell number</t>
   </si>
   <si>
     <t>Please enter a valid local number, or use the standard international format, which includes a plus sign (+) and country code. For example: +254712345678</t>
   </si>
   <si>
-    <t>Must be in the format +1 (876) xxx-xxxx</t>
+    <t>Must be in the format +1 (876) xxx-xxx</t>
   </si>
   <si>
     <t>select_one phone</t>
@@ -198,7 +204,7 @@
     <t>type1</t>
   </si>
   <si>
-    <t>Type of phone</t>
+    <t>Type of current phone</t>
   </si>
   <si>
     <t>select_one network</t>
@@ -207,7 +213,7 @@
     <t>network1</t>
   </si>
   <si>
-    <t>Which network do you use?</t>
+    <t>Which network do you currently use?</t>
   </si>
   <si>
     <t>date</t>
@@ -348,6 +354,12 @@
   </si>
   <si>
     <t>Flow</t>
+  </si>
+  <si>
+    <t>both</t>
+  </si>
+  <si>
+    <t>Both</t>
   </si>
   <si>
     <t>form_title</t>
@@ -1062,7 +1074,9 @@
       <c r="C20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
@@ -1110,120 +1124,137 @@
       <c r="C24" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="F24" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="B26" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I25" s="3" t="b">
+      <c r="I26" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="J25" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="K26" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="J29" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="3" t="s">
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="17" t="s">
+      <c r="B31" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="B32" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="3"/>
       <c r="E32" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H32" s="7"/>
     </row>
     <row r="33">
       <c r="A33" s="15" t="s">
@@ -1233,6 +1264,9 @@
         <v>80</v>
       </c>
       <c r="C33" s="3"/>
+      <c r="E33" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="G33" s="7" t="s">
         <v>81</v>
       </c>
@@ -1252,12 +1286,25 @@
       <c r="H34" s="7"/>
     </row>
     <row r="35">
-      <c r="A35" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A35" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="G35" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H35" s="7"/>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1281,7 +1328,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1292,140 +1339,146 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="21" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="21" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="7"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
+      <c r="A14" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="7"/>
@@ -1464,22 +1517,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="24"/>
@@ -1489,21 +1542,21 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C2" s="25" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-09-29_16-59</v>
+        <v>2022-10-19_10-31</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="G2" s="7"/>
     </row>

</xml_diff>

<commit_message>
auto:removing the the docket number as a required field
</commit_message>
<xml_diff>
--- a/config/forms/contact/person-create.xlsx
+++ b/config/forms/contact/person-create.xlsx
@@ -9,11 +9,16 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7miLnrLCftoNQnCqmMRkDBy7ctjKAA=="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="125">
   <si>
     <t>type</t>
   </si>
@@ -414,11 +419,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -431,6 +431,11 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -479,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -489,73 +494,44 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -780,18 +756,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="20.25"/>
     <col customWidth="1" min="2" max="2" width="22.0"/>
     <col customWidth="1" min="3" max="3" width="45.25"/>
+    <col customWidth="1" min="4" max="6" width="12.63"/>
     <col customWidth="1" min="7" max="7" width="44.63"/>
     <col customWidth="1" min="8" max="8" width="24.0"/>
     <col customWidth="1" min="10" max="10" width="116.25"/>
     <col customWidth="1" min="11" max="11" width="29.88"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -829,111 +806,111 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5" t="b">
+      <c r="D2" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="7" t="s">
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="7" t="s">
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6">
-      <c r="A6" s="7" t="s">
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7">
-      <c r="A7" s="7" t="s">
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8">
-      <c r="A8" s="7" t="s">
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="6"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9">
-      <c r="A9" s="9" t="s">
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="10" t="s">
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>27</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -943,45 +920,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="10" t="s">
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="10" t="s">
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="10" t="s">
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -989,31 +966,31 @@
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14">
-      <c r="A14" s="12" t="s">
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="6"/>
       <c r="G14" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15">
-      <c r="A15" s="7" t="s">
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="13" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -1023,26 +1000,26 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="12" t="s">
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="6" t="s">
         <v>38</v>
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18">
-      <c r="A18" s="12" t="s">
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="6" t="s">
         <v>39</v>
       </c>
       <c r="E18" s="3"/>
@@ -1050,7 +1027,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>40</v>
       </c>
@@ -1064,7 +1041,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -1074,11 +1051,9 @@
       <c r="C20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
@@ -1089,7 +1064,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
@@ -1099,26 +1074,27 @@
       <c r="C22" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="s">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="5" t="s">
+      <c r="F23" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1128,38 +1104,38 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="5" t="s">
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
-      <c r="Y25" s="5"/>
-      <c r="Z25" s="5"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="5" t="s">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -1178,7 +1154,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>61</v>
       </c>
@@ -1189,7 +1165,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>64</v>
       </c>
@@ -1200,7 +1176,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>67</v>
       </c>
@@ -1220,7 +1196,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>72</v>
       </c>
@@ -1231,7 +1207,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>75</v>
       </c>
@@ -1242,72 +1218,1035 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="17" t="s">
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="7" t="s">
         <v>78</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="15" t="s">
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="9" t="s">
         <v>80</v>
       </c>
       <c r="C33" s="3"/>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="G33" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="15" t="s">
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="9" t="s">
         <v>82</v>
       </c>
       <c r="C34" s="3"/>
-      <c r="G34" s="7" t="s">
+      <c r="G34" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H34" s="7"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="15" t="s">
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="9" t="s">
         <v>84</v>
       </c>
       <c r="C35" s="3"/>
-      <c r="G35" s="7" t="s">
+      <c r="G35" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H35" s="7"/>
-    </row>
-    <row r="36">
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1321,12 +2260,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="12.63"/>
     <col customWidth="1" min="2" max="2" width="22.38"/>
+    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
@@ -1337,7 +2278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>57</v>
       </c>
@@ -1348,7 +2289,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>57</v>
       </c>
@@ -1359,7 +2300,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>91</v>
       </c>
@@ -1370,7 +2311,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>91</v>
       </c>
@@ -1381,7 +2322,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>91</v>
       </c>
@@ -1392,7 +2333,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>98</v>
       </c>
@@ -1403,7 +2344,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>98</v>
       </c>
@@ -1414,87 +2355,1070 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="7" t="s">
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="14" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="7" t="s">
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="14" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="7" t="s">
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="14" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="21" t="s">
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="21" t="s">
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="21" t="s">
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="14" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="7"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="7"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="6"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="6"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1"/>
+    <row r="24" ht="15.75" customHeight="1"/>
+    <row r="25" ht="15.75" customHeight="1"/>
+    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1"/>
+    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1508,14 +3432,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="18.63"/>
+    <col customWidth="1" min="2" max="6" width="12.63"/>
     <col customWidth="1" min="7" max="7" width="17.75"/>
     <col customWidth="1" min="8" max="8" width="17.5"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -1531,35 +3456,1033 @@
       <c r="E1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="16" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="25" t="str">
+      <c r="C2" s="16" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-10-19_10-31</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+        <v>2022-11-29_08-16</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="7"/>
-    </row>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1"/>
+    <row r="4" ht="15.75" customHeight="1"/>
+    <row r="5" ht="15.75" customHeight="1"/>
+    <row r="6" ht="15.75" customHeight="1"/>
+    <row r="7" ht="15.75" customHeight="1"/>
+    <row r="8" ht="15.75" customHeight="1"/>
+    <row r="9" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1"/>
+    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1"/>
+    <row r="24" ht="15.75" customHeight="1"/>
+    <row r="25" ht="15.75" customHeight="1"/>
+    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1"/>
+    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
auto:add date of registration to healthjam enrollment form
</commit_message>
<xml_diff>
--- a/config/forms/contact/person-create.xlsx
+++ b/config/forms/contact/person-create.xlsx
@@ -10,15 +10,15 @@
   <definedNames/>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7miLnrLCftoNQnCqmMRkDBy7ctjKAA=="/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="mGbif54xzWwTtYyqjmxobg5ZcoERKm2bvwKtAvQJEQI="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="126">
   <si>
     <t>type</t>
   </si>
@@ -140,6 +140,15 @@
     <t>Person Type</t>
   </si>
   <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>date_reg</t>
+  </si>
+  <si>
+    <t>Date Registered into HealthJam Digital Case Management System</t>
+  </si>
+  <si>
     <t xml:space="preserve">string </t>
   </si>
   <si>
@@ -197,10 +206,7 @@
     <t>Current Cell number</t>
   </si>
   <si>
-    <t>Please enter a valid local number, or use the standard international format, which includes a plus sign (+) and country code. For example: +254712345678</t>
-  </si>
-  <si>
-    <t>Must be in the format +1 (876) xxx-xxx</t>
+    <t>Must be in the format +1 (876) xxx-xxxx</t>
   </si>
   <si>
     <t>select_one phone</t>
@@ -219,9 +225,6 @@
   </si>
   <si>
     <t>Which network do you currently use?</t>
-  </si>
-  <si>
-    <t>date</t>
   </si>
   <si>
     <t>date_of_birth</t>
@@ -319,10 +322,10 @@
     <t>gender</t>
   </si>
   <si>
-    <t>gender_male</t>
-  </si>
-  <si>
-    <t>gender_female</t>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
   <si>
     <t>place_type</t>
@@ -484,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -519,7 +522,16 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -760,7 +772,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="20.25"/>
     <col customWidth="1" min="2" max="2" width="22.0"/>
-    <col customWidth="1" min="3" max="3" width="45.25"/>
+    <col customWidth="1" min="3" max="3" width="51.88"/>
     <col customWidth="1" min="4" max="6" width="12.63"/>
     <col customWidth="1" min="7" max="7" width="44.63"/>
     <col customWidth="1" min="8" max="8" width="24.0"/>
@@ -1028,112 +1040,98 @@
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="C19" s="13" t="s">
         <v>42</v>
       </c>
+      <c r="E19" s="3"/>
+      <c r="L19" s="3"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="3"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>42</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>42</v>
+        <v>54</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
-      <c r="Y25" s="2"/>
-      <c r="Z25" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>57</v>
@@ -1141,123 +1139,135 @@
       <c r="C26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I26" s="3" t="b">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="J26" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="J27" s="3"/>
+      <c r="K27" s="15" t="s">
         <v>62</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J30" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="3" t="s">
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="8" t="s">
+      <c r="C32" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B33" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="9" t="s">
+      <c r="E33" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="E33" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H33" s="6"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="E34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="C34" s="3"/>
-      <c r="G34" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="H34" s="6"/>
     </row>
@@ -1266,25 +1276,37 @@
         <v>32</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C35" s="3"/>
       <c r="G35" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="H35" s="6"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="C36" s="3"/>
+      <c r="G36" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H36" s="6"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="39" ht="15.75" customHeight="1"/>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1"/>
@@ -2247,6 +2269,7 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2269,7 +2292,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2280,151 +2303,151 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="3" t="s">
         <v>99</v>
       </c>
+      <c r="B7" s="15" t="s">
+        <v>100</v>
+      </c>
       <c r="C7" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="B9" s="16" t="s">
         <v>103</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="C10" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>105</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>107</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="16" t="s">
         <v>110</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>112</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>114</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="6"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="6"/>
@@ -2433,8 +2456,8 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="6"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
     </row>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -3442,46 +3465,46 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1" s="15" t="s">
         <v>120</v>
       </c>
+      <c r="F1" s="18" t="s">
+        <v>121</v>
+      </c>
       <c r="G1" s="7"/>
-      <c r="H1" s="15"/>
+      <c r="H1" s="18"/>
       <c r="I1" s="7"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" s="16" t="str">
+        <v>123</v>
+      </c>
+      <c r="C2" s="19" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-11-29_08-16</v>
+        <v>2023-06-19_10-37</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G2" s="6"/>
     </row>

</xml_diff>

<commit_message>
auto:adding more context objects in the contact summary and more fields in the enrollment form
</commit_message>
<xml_diff>
--- a/config/forms/contact/person-create.xlsx
+++ b/config/forms/contact/person-create.xlsx
@@ -11,14 +11,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="mGbif54xzWwTtYyqjmxobg5ZcoERKm2bvwKtAvQJEQI="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="n3+giVEjsfrAwHVLMVKDXuj//ywRGzn2sZcpAFhMrNA="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="131">
   <si>
     <t>type</t>
   </si>
@@ -149,6 +149,15 @@
     <t>Date Registered into HealthJam Digital Case Management System</t>
   </si>
   <si>
+    <t>full_name</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>This name will be the main name used in the Digital Case Management System</t>
+  </si>
+  <si>
     <t xml:space="preserve">string </t>
   </si>
   <si>
@@ -158,10 +167,16 @@
     <t>yes</t>
   </si>
   <si>
+    <t>Must match the client’s first name in TSIS</t>
+  </si>
+  <si>
     <t>name1</t>
   </si>
   <si>
     <t>Last Name</t>
+  </si>
+  <si>
+    <t>Must match the client’s surname in TSIS</t>
   </si>
   <si>
     <t>aka</t>
@@ -528,10 +543,10 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -777,7 +792,7 @@
     <col customWidth="1" min="7" max="7" width="44.63"/>
     <col customWidth="1" min="8" max="8" width="24.0"/>
     <col customWidth="1" min="10" max="10" width="116.25"/>
-    <col customWidth="1" min="11" max="11" width="29.88"/>
+    <col customWidth="1" min="11" max="11" width="59.5"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -1053,175 +1068,176 @@
       <c r="L19" s="3"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="3"/>
+      <c r="K20" s="15" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="K22" s="15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>51</v>
+      <c r="A23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="3"/>
+        <v>54</v>
+      </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>45</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>45</v>
+        <v>59</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="V26" s="2"/>
-      <c r="W26" s="2"/>
-      <c r="Y26" s="2"/>
-      <c r="Z26" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I27" s="3" t="b">
+        <v>63</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>65</v>
+      <c r="J28" s="3"/>
+      <c r="K28" s="14" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>74</v>
@@ -1229,58 +1245,65 @@
       <c r="C31" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="F31" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B34" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="3"/>
       <c r="E34" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H34" s="6"/>
+        <v>85</v>
+      </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C35" s="3"/>
+      <c r="E35" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="G35" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H35" s="6"/>
     </row>
@@ -1289,25 +1312,37 @@
         <v>32</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C36" s="3"/>
       <c r="G36" s="6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H36" s="6"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A37" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="G37" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H37" s="6"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -2270,6 +2305,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2292,7 +2328,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2303,145 +2339,145 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
@@ -3465,22 +3501,22 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="18"/>
@@ -3490,21 +3526,21 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C2" s="19" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-06-19_10-37</v>
+        <v>2023-07-31_04-43</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G2" s="6"/>
     </row>

</xml_diff>

<commit_message>
auto:formats in the enrollment form
</commit_message>
<xml_diff>
--- a/config/forms/contact/person-create.xlsx
+++ b/config/forms/contact/person-create.xlsx
@@ -149,37 +149,37 @@
     <t>Date Registered into HealthJam Digital Case Management System</t>
   </si>
   <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>This name will be the main name used in the Digital Case Management System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string </t>
+  </si>
+  <si>
+    <t>name_f</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Must match the client’s first name in TSIS</t>
+  </si>
+  <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Must match the client’s surname in TSIS</t>
+  </si>
+  <si>
     <t>full_name</t>
-  </si>
-  <si>
-    <t>Full Name</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>This name will be the main name used in the Digital Case Management System</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string </t>
-  </si>
-  <si>
-    <t>name_f</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Must match the client’s first name in TSIS</t>
-  </si>
-  <si>
-    <t>name1</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Must match the client’s surname in TSIS</t>
   </si>
   <si>
     <t>aka</t>
@@ -1069,33 +1069,33 @@
         <v>17</v>
       </c>
       <c r="B20" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="F20" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="K20" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="C21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="F21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K21" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K21" s="15" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -1103,16 +1103,16 @@
         <v>17</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="F22" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K22" s="15" t="s">
         <v>52</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -1120,14 +1120,14 @@
         <v>32</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="15" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="K23" s="15"/>
     </row>
@@ -1165,12 +1165,12 @@
         <v>60</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>61</v>
@@ -1179,12 +1179,12 @@
         <v>62</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>63</v>
@@ -1220,7 +1220,7 @@
         <v>67</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I29" s="3" t="b">
         <v>1</v>
@@ -1263,7 +1263,7 @@
         <v>76</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>77</v>
@@ -1283,7 +1283,7 @@
         <v>81</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -3553,7 +3553,7 @@
       </c>
       <c r="C2" s="19" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-08-30_10-48</v>
+        <v>2023-09-15_04-09</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">

</xml_diff>

<commit_message>
auto:Update HealthJam Registration form
</commit_message>
<xml_diff>
--- a/config/forms/contact/person-create.xlsx
+++ b/config/forms/contact/person-create.xlsx
@@ -11,14 +11,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="HTSC0uoOpa+UBeBr9GUuFQNsFJ1H5/GmAcdGeOUz3yk="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="vb7hOnxo+2PrGDoYhBy++bY3ZYfsW9sVRwNciAo5HnE="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="129">
   <si>
     <t>type</t>
   </si>
@@ -41,6 +41,9 @@
     <t>calculation</t>
   </si>
   <si>
+    <t>hint::en</t>
+  </si>
+  <si>
     <t>read_only</t>
   </si>
   <si>
@@ -50,9 +53,6 @@
     <t>constraint_message</t>
   </si>
   <si>
-    <t>hint::en</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
@@ -149,13 +149,14 @@
     <t>Date Registered into HealthJam Digital Case Management System</t>
   </si>
   <si>
-    <t>Full Name</t>
+    <t>Preferred Name</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
-    <t>This name will be the main name used in the Digital Case Management System</t>
+    <t xml:space="preserve">
+This name will display in HealthJam</t>
   </si>
   <si>
     <t xml:space="preserve">string </t>
@@ -182,12 +183,6 @@
     <t>full_name</t>
   </si>
   <si>
-    <t>aka</t>
-  </si>
-  <si>
-    <t>Also Known as:</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
@@ -221,7 +216,7 @@
     <t>phone</t>
   </si>
   <si>
-    <t>Current Cell number</t>
+    <t>Cell number</t>
   </si>
   <si>
     <t>Must be in the format +1 (876) xxx-xxxx</t>
@@ -233,7 +228,10 @@
     <t>type1</t>
   </si>
   <si>
-    <t>Type of current phone</t>
+    <t xml:space="preserve">Phone Type </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>select_one network</t>
@@ -784,12 +782,12 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="20.25"/>
     <col customWidth="1" min="2" max="2" width="22.0"/>
-    <col customWidth="1" min="3" max="3" width="51.88"/>
+    <col customWidth="1" min="3" max="3" width="34.88"/>
     <col customWidth="1" min="4" max="6" width="12.63"/>
-    <col customWidth="1" min="7" max="7" width="44.63"/>
-    <col customWidth="1" min="8" max="8" width="24.0"/>
-    <col customWidth="1" min="10" max="10" width="116.25"/>
-    <col customWidth="1" min="11" max="11" width="59.5"/>
+    <col customWidth="1" min="7" max="7" width="16.38"/>
+    <col customWidth="1" min="8" max="8" width="33.63"/>
+    <col customWidth="1" min="9" max="9" width="24.0"/>
+    <col customWidth="1" min="11" max="11" width="16.5"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -817,10 +815,10 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
@@ -940,7 +938,7 @@
       <c r="G10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="3" t="b">
+      <c r="I10" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -988,7 +986,7 @@
       <c r="G13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="10" t="s">
@@ -1001,7 +999,7 @@
       <c r="G14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="6" t="s">
@@ -1077,7 +1075,7 @@
       <c r="F20" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K20" s="15" t="s">
+      <c r="H20" s="15" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1094,7 +1092,7 @@
       <c r="F21" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K21" s="15" t="s">
+      <c r="H21" s="15" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1111,7 +1109,7 @@
       <c r="F22" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K22" s="15" t="s">
+      <c r="H22" s="15" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1129,22 +1127,25 @@
       <c r="G23" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="K23" s="15"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="B24" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="C24" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>57</v>
@@ -1152,11 +1153,13 @@
       <c r="C25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="3"/>
+      <c r="F25" s="15" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>59</v>
@@ -1164,7 +1167,7 @@
       <c r="C26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1178,191 +1181,181 @@
       <c r="C27" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="V28" s="2"/>
-      <c r="W28" s="2"/>
-      <c r="Y28" s="2"/>
-      <c r="Z28" s="2"/>
+      <c r="C28" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J28" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" s="3"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="A29" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I29" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J29" s="3"/>
-      <c r="K29" s="12" t="s">
+      <c r="B29" s="3" t="s">
         <v>68</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F32" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>83</v>
+      <c r="A34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>84</v>
+        <v>14</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="A35" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="3"/>
       <c r="E35" s="6" t="s">
-        <v>86</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I35" s="6"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C36" s="3"/>
-      <c r="E36" s="6" t="s">
-        <v>16</v>
-      </c>
       <c r="G36" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H36" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="I36" s="6"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C37" s="3"/>
       <c r="G37" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H37" s="6"/>
+        <v>91</v>
+      </c>
+      <c r="I37" s="6"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="G38" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H38" s="6"/>
+      <c r="A38" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
+    <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1"/>
@@ -2325,7 +2318,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
     <row r="1002" ht="15.75" customHeight="1"/>
-    <row r="1003" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2348,7 +2340,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2359,145 +2351,145 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="C9" s="17" t="s">
         <v>107</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>109</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>111</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="C12" s="17" t="s">
         <v>114</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>116</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B14" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>118</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
@@ -3521,22 +3513,22 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="18" t="s">
         <v>124</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>125</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="18"/>
@@ -3546,21 +3538,21 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>127</v>
       </c>
       <c r="C2" s="19" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-09-15_04-09</v>
+        <v>2024-11-21_09-19</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="G2" s="6"/>
     </row>

</xml_diff>

<commit_message>
auto:update the app settings
</commit_message>
<xml_diff>
--- a/config/forms/contact/person-create.xlsx
+++ b/config/forms/contact/person-create.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="129">
   <si>
     <t>type</t>
   </si>
@@ -1153,9 +1153,7 @@
       <c r="C25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="15" t="s">
-        <v>44</v>
-      </c>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
@@ -3545,7 +3543,7 @@
       </c>
       <c r="C2" s="19" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2024-11-21_09-19</v>
+        <v>2024-11-21_22-45</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">

</xml_diff>